<commit_message>
updated arua org units sheet
</commit_message>
<xml_diff>
--- a/arua_org_units.xlsx
+++ b/arua_org_units.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="396">
   <si>
     <t xml:space="preserve">County</t>
   </si>
@@ -1034,6 +1035,180 @@
   </si>
   <si>
     <t xml:space="preserve">Yapi central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adravu2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anakawa Orobi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barracks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calebe Bako </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ombavu3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ondovu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onyavu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eceko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adrivu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebira A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ombavu2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onzivu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Osoko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjumani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzuva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cekoru A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cekoru B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egara A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egara B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walaba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aciba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alukuru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anyavu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ejako</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elivu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esoko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orapi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tisi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anguru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drazini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebira B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obayiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ombatika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulupi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambala2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ndiriba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyirivu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odivu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oleni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ombarana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yivu2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aliba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ayizeveku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odruvu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ojepi A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onyai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pauduru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yiba</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1172,6 +1347,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1191,8 +1374,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G6 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14253,4 +14436,1153 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E66"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>